<commit_message>
Added Coulomb Potential, but it is slow; I don't know why, I am going to try and parallelize Lanczos
</commit_message>
<xml_diff>
--- a/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
+++ b/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="12760" yWindow="1480" windowWidth="28920" windowHeight="16000" tabRatio="500" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="11880" yWindow="3940" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -13,7 +13,7 @@
     <sheet name="FreeParticle" sheetId="4" r:id="rId4"/>
     <sheet name="FreeRotor" sheetId="5" r:id="rId5"/>
     <sheet name="RotationlessHarmonicOscillator" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet3" sheetId="7" r:id="rId7"/>
+    <sheet name="RotationlessCoulombPotential" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -204,9 +204,6 @@
     <t>l_max = 2 - 1000 iterations</t>
   </si>
   <si>
-    <t>l_max = 6 - 1000 iterations</t>
-  </si>
-  <si>
     <t>B=</t>
   </si>
   <si>
@@ -231,7 +228,22 @@
     <t>Doesn't work; v is always 0</t>
   </si>
   <si>
-    <t>l_max = 20 - 1000 iterations</t>
+    <t>Ideal: E = -Z^2/2n^2 * m * (e^2/4pi.Eps0.hbar)</t>
+  </si>
+  <si>
+    <t>V(r) = -1/4pi.eps0 * Ze^2/r</t>
+  </si>
+  <si>
+    <t>l_max = 20 - 10000 iterations</t>
+  </si>
+  <si>
+    <t>l_max = 6 - 5000 iterations</t>
+  </si>
+  <si>
+    <t>Note: There are extra eigenvalues, see files in folder FreeRotor_2013-07-22_17_33_12; these are nearly equal to those present.</t>
+  </si>
+  <si>
+    <t>Note: the more iterations, the fewer the near degenerate eigenvalues, or so it seems</t>
   </si>
 </sst>
 </file>
@@ -241,7 +253,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,6 +273,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -550,7 +569,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -567,6 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="253">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -8028,7 +8048,7 @@
         <v>1</v>
       </c>
       <c r="D101">
-        <f t="shared" ref="D101:D132" si="20">LOOKUP(A101,$L$4:$L$13,$M$4:$M$13)+LOOKUP(B101,$L$4:$L$13,$M$4:$M$13)+LOOKUP(C101,$L$4:$L$13,$M$4:$M$13)</f>
+        <f t="shared" ref="D101:D129" si="20">LOOKUP(A101,$L$4:$L$13,$M$4:$M$13)+LOOKUP(B101,$L$4:$L$13,$M$4:$M$13)+LOOKUP(C101,$L$4:$L$13,$M$4:$M$13)</f>
         <v>0.38399925601279999</v>
       </c>
       <c r="E101">
@@ -56939,7 +56959,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -56949,7 +56969,7 @@
         <v>54</v>
       </c>
       <c r="J1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -56957,20 +56977,20 @@
         <v>36</v>
       </c>
       <c r="J2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>0.709652722117881</v>
@@ -56979,7 +56999,17 @@
         <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="N5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="N6" s="12" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -56996,17 +57026,17 @@
       </c>
       <c r="I7" s="6"/>
       <c r="K7" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="L7" s="6"/>
       <c r="N7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>55</v>
@@ -57063,7 +57093,7 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" t="e">
         <f>B9-C9</f>
@@ -57095,18 +57125,23 @@
         <f>$B$4*$A9*($A9+1)</f>
         <v>0</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="6">
+        <v>-2.01620196186366E-9</v>
+      </c>
       <c r="M9">
         <f>K9-L9</f>
-        <v>0</v>
+        <v>2.01620196186366E-9</v>
       </c>
       <c r="N9">
         <f>$B$4*$A9*($A9+1)</f>
         <v>0</v>
       </c>
+      <c r="O9" s="6">
+        <v>-9.8191534902980394E-9</v>
+      </c>
       <c r="P9">
         <f>N9-O9</f>
-        <v>0</v>
+        <v>9.8191534902980394E-9</v>
       </c>
     </row>
     <row r="10" spans="1:16">
@@ -57139,18 +57174,23 @@
         <f t="shared" ref="K10:K15" si="0">$B$4*$A10*($A10+1)</f>
         <v>1.419305444235762</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="6">
+        <v>1.4193054439871999</v>
+      </c>
       <c r="M10">
         <f t="shared" ref="M10:M15" si="1">K10-L10</f>
-        <v>1.419305444235762</v>
+        <v>2.4856205982359825E-10</v>
       </c>
       <c r="N10">
         <f t="shared" ref="N10:N29" si="2">$B$4*$A10*($A10+1)</f>
         <v>1.419305444235762</v>
       </c>
+      <c r="O10" s="6">
+        <v>1.41930544264287</v>
+      </c>
       <c r="P10">
-        <f t="shared" ref="P10:P15" si="3">N10-O10</f>
-        <v>1.419305444235762</v>
+        <f t="shared" ref="P10:P29" si="3">N10-O10</f>
+        <v>1.5928920404917335E-9</v>
       </c>
     </row>
     <row r="11" spans="1:16">
@@ -57172,18 +57212,23 @@
         <f t="shared" si="0"/>
         <v>4.2579163327072855</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="6">
+        <v>4.2579163320574898</v>
+      </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>4.2579163327072855</v>
+        <v>6.4979577274471012E-10</v>
       </c>
       <c r="N11">
         <f t="shared" si="2"/>
         <v>4.2579163327072855</v>
       </c>
+      <c r="O11" s="6">
+        <v>4.25791631735461</v>
+      </c>
       <c r="P11">
         <f t="shared" si="3"/>
-        <v>4.2579163327072855</v>
+        <v>1.5352675575286412E-8</v>
       </c>
     </row>
     <row r="12" spans="1:16">
@@ -57194,18 +57239,23 @@
         <f t="shared" si="0"/>
         <v>8.5158326654145711</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="6">
+        <v>8.5158326653317609</v>
+      </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>8.5158326654145711</v>
+        <v>8.2810203139160876E-11</v>
       </c>
       <c r="N12">
         <f t="shared" si="2"/>
         <v>8.5158326654145711</v>
       </c>
+      <c r="O12" s="6">
+        <v>8.5158326594321903</v>
+      </c>
       <c r="P12">
         <f t="shared" si="3"/>
-        <v>8.5158326654145711</v>
+        <v>5.9823808129522149E-9</v>
       </c>
     </row>
     <row r="13" spans="1:16">
@@ -57216,18 +57266,23 @@
         <f t="shared" si="0"/>
         <v>14.193054442357621</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="6">
+        <v>14.1930544407748</v>
+      </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>14.193054442357621</v>
+        <v>1.5828209853907538E-9</v>
       </c>
       <c r="N13">
         <f t="shared" si="2"/>
         <v>14.193054442357621</v>
       </c>
+      <c r="O13" s="6">
+        <v>14.193054438550901</v>
+      </c>
       <c r="P13">
         <f t="shared" si="3"/>
-        <v>14.193054442357621</v>
+        <v>3.8067202723368609E-9</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -57238,18 +57293,23 @@
         <f t="shared" si="0"/>
         <v>21.289581663536431</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="6">
+        <v>21.289581662865501</v>
+      </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>21.289581663536431</v>
+        <v>6.709299782414746E-10</v>
       </c>
       <c r="N14">
         <f t="shared" si="2"/>
         <v>21.289581663536431</v>
       </c>
+      <c r="O14" s="6">
+        <v>21.289581632626899</v>
+      </c>
       <c r="P14">
         <f t="shared" si="3"/>
-        <v>21.289581663536431</v>
+        <v>3.0909532711120846E-8</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -57260,32 +57320,42 @@
         <f t="shared" si="0"/>
         <v>29.805414328950999</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="6">
+        <v>29.805414328818099</v>
+      </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>29.805414328950999</v>
+        <v>1.3289991329656914E-10</v>
       </c>
       <c r="N15">
         <f t="shared" si="2"/>
         <v>29.805414328950999</v>
       </c>
+      <c r="O15" s="6">
+        <v>29.8054143206435</v>
+      </c>
       <c r="P15">
         <f t="shared" si="3"/>
-        <v>29.805414328950999</v>
+        <v>8.3074986889641877E-9</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16">
         <v>7</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="6">
+        <v>29.805414332045402</v>
+      </c>
       <c r="N16">
         <f t="shared" si="2"/>
         <v>39.740552438601334</v>
       </c>
+      <c r="O16" s="6">
+        <v>39.740552433134702</v>
+      </c>
       <c r="P16">
-        <f t="shared" ref="P16:P29" si="4">N16-O16</f>
-        <v>39.740552438601334</v>
+        <f t="shared" si="3"/>
+        <v>5.4666315918439068E-9</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -57297,9 +57367,12 @@
         <f t="shared" si="2"/>
         <v>51.094995992487434</v>
       </c>
+      <c r="O17" s="6">
+        <v>51.094995974433502</v>
+      </c>
       <c r="P17">
-        <f t="shared" si="4"/>
-        <v>51.094995992487434</v>
+        <f t="shared" si="3"/>
+        <v>1.805393168297087E-8</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -57311,9 +57384,12 @@
         <f t="shared" si="2"/>
         <v>63.868744990609294</v>
       </c>
+      <c r="O18" s="6">
+        <v>63.868744966188203</v>
+      </c>
       <c r="P18">
-        <f t="shared" si="4"/>
-        <v>63.868744990609294</v>
+        <f t="shared" si="3"/>
+        <v>2.4421090927262412E-8</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -57325,9 +57401,12 @@
         <f t="shared" si="2"/>
         <v>78.061799432966922</v>
       </c>
+      <c r="O19" s="6">
+        <v>78.061799413655805</v>
+      </c>
       <c r="P19">
-        <f t="shared" si="4"/>
-        <v>78.061799432966922</v>
+        <f t="shared" si="3"/>
+        <v>1.9311116261633288E-8</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -57339,9 +57418,12 @@
         <f t="shared" si="2"/>
         <v>93.674159319560289</v>
       </c>
+      <c r="O20" s="6">
+        <v>93.674159293629103</v>
+      </c>
       <c r="P20">
-        <f t="shared" si="4"/>
-        <v>93.674159319560289</v>
+        <f t="shared" si="3"/>
+        <v>2.593118608729128E-8</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -57353,9 +57435,12 @@
         <f t="shared" si="2"/>
         <v>110.70582465038942</v>
       </c>
+      <c r="O21" s="6">
+        <v>110.705824645981</v>
+      </c>
       <c r="P21">
-        <f t="shared" si="4"/>
-        <v>110.70582465038942</v>
+        <f t="shared" si="3"/>
+        <v>4.4084202954763896E-9</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -57366,9 +57451,12 @@
         <f t="shared" si="2"/>
         <v>129.15679542545433</v>
       </c>
+      <c r="O22" s="6">
+        <v>129.15679537149899</v>
+      </c>
       <c r="P22">
-        <f t="shared" si="4"/>
-        <v>129.15679542545433</v>
+        <f t="shared" si="3"/>
+        <v>5.3955346857037512E-8</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -57379,9 +57467,12 @@
         <f t="shared" si="2"/>
         <v>149.02707164475501</v>
       </c>
+      <c r="O23" s="6">
+        <v>149.027071641844</v>
+      </c>
       <c r="P23">
-        <f t="shared" si="4"/>
-        <v>149.02707164475501</v>
+        <f t="shared" si="3"/>
+        <v>2.9110083232808392E-9</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -57392,9 +57483,12 @@
         <f t="shared" si="2"/>
         <v>170.31665330829145</v>
       </c>
+      <c r="O24" s="6">
+        <v>170.316653272086</v>
+      </c>
       <c r="P24">
-        <f t="shared" si="4"/>
-        <v>170.31665330829145</v>
+        <f t="shared" si="3"/>
+        <v>3.6205449305271031E-8</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -57405,9 +57499,12 @@
         <f t="shared" si="2"/>
         <v>193.02554041606362</v>
       </c>
+      <c r="O25" s="6">
+        <v>193.02554039567099</v>
+      </c>
       <c r="P25">
-        <f t="shared" si="4"/>
-        <v>193.02554041606362</v>
+        <f t="shared" si="3"/>
+        <v>2.0392633359733736E-8</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -57418,9 +57515,12 @@
         <f t="shared" si="2"/>
         <v>217.15373296807158</v>
       </c>
+      <c r="O26" s="6">
+        <v>217.15373296807201</v>
+      </c>
       <c r="P26">
-        <f t="shared" si="4"/>
-        <v>217.15373296807158</v>
+        <f t="shared" si="3"/>
+        <v>-4.2632564145606011E-13</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -57431,9 +57531,12 @@
         <f t="shared" si="2"/>
         <v>242.7012309643153</v>
       </c>
+      <c r="O27" s="6">
+        <v>242.701230964286</v>
+      </c>
       <c r="P27">
-        <f t="shared" si="4"/>
-        <v>242.7012309643153</v>
+        <f t="shared" si="3"/>
+        <v>2.9302782422746532E-11</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -57444,9 +57547,12 @@
         <f t="shared" si="2"/>
         <v>269.66803440479475</v>
       </c>
+      <c r="O28" s="6">
+        <v>269.668034344749</v>
+      </c>
       <c r="P28">
-        <f t="shared" si="4"/>
-        <v>269.66803440479475</v>
+        <f t="shared" si="3"/>
+        <v>6.0045749705750495E-8</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -57457,9 +57563,12 @@
         <f t="shared" si="2"/>
         <v>298.05414328951002</v>
       </c>
+      <c r="O29" s="6">
+        <v>298.05414328634703</v>
+      </c>
       <c r="P29">
-        <f t="shared" si="4"/>
-        <v>298.05414328951002</v>
+        <f t="shared" si="3"/>
+        <v>3.1629951990908012E-9</v>
       </c>
     </row>
   </sheetData>
@@ -57492,12 +57601,25 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
Tested Parallelization of Lanczos Loop, all attempts have no statistically significant improvement
</commit_message>
<xml_diff>
--- a/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
+++ b/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11880" yWindow="3940" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="4940" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="FreeRotor" sheetId="5" r:id="rId5"/>
     <sheet name="RotationlessHarmonicOscillator" sheetId="6" r:id="rId6"/>
     <sheet name="RotationlessCoulombPotential" sheetId="7" r:id="rId7"/>
+    <sheet name="TimingLanczosParallelization" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -245,13 +246,98 @@
   <si>
     <t>Note: the more iterations, the fewer the near degenerate eigenvalues, or so it seems</t>
   </si>
+  <si>
+    <t>Z =</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">e = </t>
+  </si>
+  <si>
+    <t>PI =</t>
+  </si>
+  <si>
+    <t>eps0 =</t>
+  </si>
+  <si>
+    <t>h_bar =</t>
+  </si>
+  <si>
+    <t>kJ/mol.ps</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>None:</t>
+  </si>
+  <si>
+    <t>1st Loop:</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>T3</t>
+  </si>
+  <si>
+    <t>Avg</t>
+  </si>
+  <si>
+    <t>RSD</t>
+  </si>
+  <si>
+    <t>Std Dev</t>
+  </si>
+  <si>
+    <t>95% CI, T-dist</t>
+  </si>
+  <si>
+    <t>2nd Loop:</t>
+  </si>
+  <si>
+    <t>4th Loop:</t>
+  </si>
+  <si>
+    <t>T4</t>
+  </si>
+  <si>
+    <t>Toby (1000 iterations):</t>
+  </si>
+  <si>
+    <t>Mac (1000 iterations):</t>
+  </si>
+  <si>
+    <t>6th Loop:</t>
+  </si>
+  <si>
+    <t>7th Loop:</t>
+  </si>
+  <si>
+    <t>8th Loop:</t>
+  </si>
+  <si>
+    <t>None (after):</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.00000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -314,7 +400,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="253">
+  <cellStyleXfs count="259">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -568,8 +654,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -587,8 +679,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="253">
+  <cellStyles count="259">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -715,6 +809,9 @@
     <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -841,11 +938,307 @@
     <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Effect of Lanczos Loop Parallelization</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="1"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>TimingLanczosParallelization!$I$14:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.0417070485706302</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15960095137594</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.115092669407768</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0480253361511355</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00912933227292609</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.0549375410519272</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.124112005810021</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.0259357984507788</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>TimingLanczosParallelization!$I$14:$I$21</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="8"/>
+                  <c:pt idx="0">
+                    <c:v>0.0417070485706302</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15960095137594</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.115092669407768</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.0480253361511355</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.00912933227292609</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.0549375410519272</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.124112005810021</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.0259357984507788</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>TimingLanczosParallelization!$A$14:$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>None:</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1st Loop:</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2nd Loop:</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4th Loop:</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6th Loop:</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7th Loop:</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8th Loop:</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>None (after):</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TimingLanczosParallelization!$F$14:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>5.871</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.02125</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.99875</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.90975</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.893750000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9785</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.9125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="10"/>
+        <c:axId val="519670776"/>
+        <c:axId val="571390920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="519670776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="571390920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="571390920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="519670776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -56958,7 +57351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P29"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+    <sheetView showRuler="0" workbookViewId="0">
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
@@ -57601,22 +57994,703 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:A4"/>
+  <dimension ref="A3:C81"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7">
+        <v>2.0156500639999999</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9">
+        <v>3.14159265358979</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>5.7276563844481799E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11">
+        <v>6.3507785700200006E-2</v>
+      </c>
+      <c r="C11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <f>1</f>
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <f>-1*$B$6*$B$6/2/(A14*A14) *$B$7 * $B$8*$B$8 / 4 / $B$9 /$B$10 / $B$11</f>
+        <v>-2204.8109169665272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <f>-1*$B$6*$B$6/2/(A15*A15) *$B$7 * $B$8*$B$8 / 4 / $B$9 /$B$10 / $B$11</f>
+        <v>-551.2027292416318</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <f t="shared" ref="B16:B79" si="0">-1*$B$6*$B$6/2/(A16*A16) *$B$7 * $B$8*$B$8 / 4 / $B$9 /$B$10 / $B$11</f>
+        <v>-244.97899077405859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>-137.80068231040795</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>-88.192436678661082</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19">
+        <v>6</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>-61.244747693514647</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20">
+        <v>7</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>-44.996141162582191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>8</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>-34.450170577601988</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22">
+        <v>9</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>-27.219887863784283</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23">
+        <v>10</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>-22.04810916966527</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24">
+        <v>11</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>-18.221577826169646</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25">
+        <v>12</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>-15.311186923378662</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26">
+        <v>13</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>-13.046218443588918</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>-11.249035290645548</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28">
+        <v>15</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>-9.7991596309623432</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>16</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>-8.6125426444004969</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30">
+        <v>17</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>-7.6291035189153202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31">
+        <v>18</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>-6.8049719659460708</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>-6.1075094652812387</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>-5.5120272924163176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34">
+        <v>21</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>-4.9995712402869108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>22</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>-4.5553944565424116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36">
+        <v>23</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>-4.1678845311276511</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37">
+        <v>24</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>-3.8277967308446654</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38">
+        <v>25</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>-3.5276974671464436</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>26</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>-3.2615546108972295</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40">
+        <v>27</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>-3.024431984864921</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>-2.8122588226613869</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42">
+        <v>29</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>-2.6216538846213164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>30</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>-2.4497899077405858</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44">
+        <v>31</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>-2.2942881550119947</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45">
+        <v>32</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>-2.1531356611001242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>-2.0246197584632943</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47">
+        <v>34</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>-1.9072758797288301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48">
+        <v>35</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>-1.7998456465032877</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49">
+        <v>36</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>-1.7012429914865177</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50">
+        <v>37</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>-1.6105266011442858</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51">
+        <v>38</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>-1.5268773663203097</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52">
+        <v>39</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>-1.4495798270654354</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53">
+        <v>40</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>-1.3780068231040794</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54">
+        <v>41</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>-1.3116067322822886</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55">
+        <v>42</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>-1.2498928100717277</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56">
+        <v>43</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>-1.1924342438975268</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57">
+        <v>44</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>-1.1388486141356029</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58">
+        <v>45</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>-1.0887955145513715</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59">
+        <v>46</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>-1.0419711327819128</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60">
+        <v>47</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>-0.99810362922884888</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61">
+        <v>48</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>-0.95694918271116636</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62">
+        <v>49</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>-0.91828859515473849</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63">
+        <v>50</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>-0.8819243667866109</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64">
+        <v>51</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>-0.84767816876836877</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65">
+        <v>52</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>-0.81538865272430738</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66">
+        <v>53</v>
+      </c>
+      <c r="B66">
+        <f t="shared" si="0"/>
+        <v>-0.78490954680189662</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67">
+        <v>54</v>
+      </c>
+      <c r="B67">
+        <f t="shared" si="0"/>
+        <v>-0.75610799621623026</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68">
+        <v>55</v>
+      </c>
+      <c r="B68">
+        <f t="shared" si="0"/>
+        <v>-0.72886311304678586</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69">
+        <v>56</v>
+      </c>
+      <c r="B69">
+        <f t="shared" si="0"/>
+        <v>-0.70306470566534673</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70">
+        <v>57</v>
+      </c>
+      <c r="B70">
+        <f t="shared" si="0"/>
+        <v>-0.67861216280902648</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71">
+        <v>58</v>
+      </c>
+      <c r="B71">
+        <f>-1*$B$6*$B$6/2/(A71*A71) *$B$7 * $B$8*$B$8 / 4 / $B$9 /$B$10 / $B$11</f>
+        <v>-0.65541347115532911</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72">
+        <v>59</v>
+      </c>
+      <c r="B72">
+        <f t="shared" si="0"/>
+        <v>-0.63338434845346947</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73">
+        <v>60</v>
+      </c>
+      <c r="B73">
+        <f t="shared" si="0"/>
+        <v>-0.61244747693514645</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74">
+        <v>61</v>
+      </c>
+      <c r="B74">
+        <f t="shared" si="0"/>
+        <v>-0.59253182396305482</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75">
+        <v>62</v>
+      </c>
+      <c r="B75">
+        <f t="shared" si="0"/>
+        <v>-0.57357203875299867</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76">
+        <v>63</v>
+      </c>
+      <c r="B76">
+        <f t="shared" si="0"/>
+        <v>-0.5555079155874344</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77">
+        <v>64</v>
+      </c>
+      <c r="B77">
+        <f t="shared" si="0"/>
+        <v>-0.53828391527503106</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78">
+        <v>65</v>
+      </c>
+      <c r="B78">
+        <f t="shared" si="0"/>
+        <v>-0.52184873774355678</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79">
+        <v>66</v>
+      </c>
+      <c r="B79">
+        <f t="shared" si="0"/>
+        <v>-0.50615493961582358</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80">
+        <v>67</v>
+      </c>
+      <c r="B80">
+        <f t="shared" ref="B80:B81" si="1">-1*$B$6*$B$6/2/(A80*A80) *$B$7 * $B$8*$B$8 / 4 / $B$9 /$B$10 / $B$11</f>
+        <v>-0.49115859143829971</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81">
+        <v>68</v>
+      </c>
+      <c r="B81">
+        <f t="shared" si="1"/>
+        <v>-0.47681896993220751</v>
       </c>
     </row>
   </sheetData>
@@ -57627,4 +58701,551 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="13">
+        <v>7.5880000000000001</v>
+      </c>
+      <c r="C3" s="13">
+        <v>6.3140000000000001</v>
+      </c>
+      <c r="D3">
+        <v>6.2160000000000002</v>
+      </c>
+      <c r="F3" s="13">
+        <f>AVERAGE(B3:D3)</f>
+        <v>6.7060000000000004</v>
+      </c>
+      <c r="G3" s="13">
+        <f>STDEV(B3:D3)</f>
+        <v>0.76540446823885211</v>
+      </c>
+      <c r="H3" s="14">
+        <f t="shared" ref="H3:H4" si="0">G3/F3</f>
+        <v>0.11413726039947093</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I10" si="1">_xlfn.T.INV.2T(0.05, COUNT(B3:E3)-1)*G3/SQRT(COUNT(B3:E3))</f>
+        <v>1.9013701042943409</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" s="13">
+        <v>8.0449999999999999</v>
+      </c>
+      <c r="C4" s="13">
+        <v>10.086</v>
+      </c>
+      <c r="D4" s="13">
+        <v>9.3800000000000008</v>
+      </c>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13">
+        <f>AVERAGE(B4:D4)</f>
+        <v>9.1703333333333337</v>
+      </c>
+      <c r="G4" s="13">
+        <f>STDEV(B4:D4)</f>
+        <v>1.0365280185954135</v>
+      </c>
+      <c r="H4" s="14">
+        <f t="shared" si="0"/>
+        <v>0.11303057161812513</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>2.574878340278715</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5">
+        <v>7.3360000000000003</v>
+      </c>
+      <c r="C5">
+        <v>7.7709999999999999</v>
+      </c>
+      <c r="D5">
+        <v>6.6289999999999996</v>
+      </c>
+      <c r="E5">
+        <v>8.3059999999999992</v>
+      </c>
+      <c r="F5" s="13">
+        <f>AVERAGE(B5:E5)</f>
+        <v>7.5104999999999986</v>
+      </c>
+      <c r="G5" s="13">
+        <f>STDEV(B5:E5)</f>
+        <v>0.70903055881487442</v>
+      </c>
+      <c r="H5" s="14">
+        <f t="shared" ref="H5:H7" si="2">G5/F5</f>
+        <v>9.4405240505275892E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>1.1282258411168204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6">
+        <v>6.6529999999999996</v>
+      </c>
+      <c r="C6">
+        <v>6.8810000000000002</v>
+      </c>
+      <c r="D6">
+        <v>9.1470000000000002</v>
+      </c>
+      <c r="E6">
+        <v>5.3940000000000001</v>
+      </c>
+      <c r="F6" s="13">
+        <f>AVERAGE(B6:E6)</f>
+        <v>7.0187499999999989</v>
+      </c>
+      <c r="G6" s="13">
+        <f>STDEV(B6:E6)</f>
+        <v>1.5622642488815248</v>
+      </c>
+      <c r="H6" s="14">
+        <f t="shared" si="2"/>
+        <v>0.22258439877207836</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>2.485911043364919</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="F7" s="13" t="e">
+        <f t="shared" ref="F7:F10" si="3">AVERAGE(B7:D7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G7" s="13" t="e">
+        <f t="shared" ref="G7:G10" si="4">STDEV(B7:D7)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H7" s="14" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I7" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="F8" s="13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G8" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H8" s="14" t="e">
+        <f t="shared" ref="H8:H10" si="5">G8/F8</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I8" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="F9" s="13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G9" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H9" s="14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I9" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="F10" s="13" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G10" s="13" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="H10" s="14" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I10" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" t="s">
+        <v>86</v>
+      </c>
+      <c r="D13" t="s">
+        <v>87</v>
+      </c>
+      <c r="E13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G13" t="s">
+        <v>90</v>
+      </c>
+      <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="13">
+        <v>5.8490000000000002</v>
+      </c>
+      <c r="C14" s="13">
+        <v>5.9</v>
+      </c>
+      <c r="D14" s="13">
+        <v>5.8639999999999999</v>
+      </c>
+      <c r="E14" s="13">
+        <v>5.8470000000000004</v>
+      </c>
+      <c r="F14" s="13">
+        <f>AVERAGE(B14:D14)</f>
+        <v>5.8709999999999996</v>
+      </c>
+      <c r="G14" s="13">
+        <f>STDEV(B14:D14)</f>
+        <v>2.6210684844162443E-2</v>
+      </c>
+      <c r="H14" s="14">
+        <f t="shared" ref="H14:H21" si="6">G14/F14</f>
+        <v>4.4644327787706425E-3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ref="I14:I21" si="7">_xlfn.T.INV.2T(0.05, COUNT(B14:E14)-1)*G14/SQRT(COUNT(B14:E14))</f>
+        <v>4.1707048570630241E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="13">
+        <v>6.1559999999999997</v>
+      </c>
+      <c r="C15" s="13">
+        <v>6.0369999999999999</v>
+      </c>
+      <c r="D15" s="13">
+        <v>5.931</v>
+      </c>
+      <c r="E15" s="13">
+        <v>5.9610000000000003</v>
+      </c>
+      <c r="F15" s="13">
+        <f>AVERAGE(B15:E15)</f>
+        <v>6.0212500000000002</v>
+      </c>
+      <c r="G15" s="13">
+        <f>STDEV(B15:E15)</f>
+        <v>0.1003007976040069</v>
+      </c>
+      <c r="H15" s="14">
+        <f t="shared" si="6"/>
+        <v>1.6657803214283895E-2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="7"/>
+        <v>0.15960095137594044</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="13">
+        <v>5.8979999999999997</v>
+      </c>
+      <c r="C16" s="13">
+        <v>6.0620000000000003</v>
+      </c>
+      <c r="D16" s="13">
+        <v>5.9969999999999999</v>
+      </c>
+      <c r="E16" s="13">
+        <v>6.0380000000000003</v>
+      </c>
+      <c r="F16" s="13">
+        <f>AVERAGE(B16:E16)</f>
+        <v>5.9987500000000002</v>
+      </c>
+      <c r="G16" s="13">
+        <f>STDEV(B16:E16)</f>
+        <v>7.2329685007840122E-2</v>
+      </c>
+      <c r="H16" s="14">
+        <f t="shared" si="6"/>
+        <v>1.2057459472030026E-2</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="7"/>
+        <v>0.11509266940776765</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" s="13">
+        <v>5.95</v>
+      </c>
+      <c r="C17" s="13">
+        <v>5.915</v>
+      </c>
+      <c r="D17" s="13">
+        <v>5.8920000000000003</v>
+      </c>
+      <c r="E17" s="13">
+        <v>5.8819999999999997</v>
+      </c>
+      <c r="F17" s="13">
+        <f>AVERAGE(B17:E17)</f>
+        <v>5.9097500000000007</v>
+      </c>
+      <c r="G17" s="13">
+        <f>STDEV(B17:E17)</f>
+        <v>3.018139603574814E-2</v>
+      </c>
+      <c r="H17" s="14">
+        <f t="shared" si="6"/>
+        <v>5.1070512349504016E-3</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="7"/>
+        <v>4.8025336151135523E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>97</v>
+      </c>
+      <c r="B18" s="13">
+        <v>5.891</v>
+      </c>
+      <c r="C18" s="13">
+        <v>5.8890000000000002</v>
+      </c>
+      <c r="D18" s="13">
+        <v>5.8929999999999998</v>
+      </c>
+      <c r="E18" s="13">
+        <v>5.9020000000000001</v>
+      </c>
+      <c r="F18" s="13">
+        <f>AVERAGE(B18:E18)</f>
+        <v>5.8937500000000007</v>
+      </c>
+      <c r="G18" s="13">
+        <f>STDEV(B18:E18)</f>
+        <v>5.7373048260195084E-3</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" si="6"/>
+        <v>9.7345574990786977E-4</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>9.1293322729260884E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>98</v>
+      </c>
+      <c r="B19" s="13">
+        <v>5.9820000000000002</v>
+      </c>
+      <c r="C19" s="13">
+        <v>5.9880000000000004</v>
+      </c>
+      <c r="D19" s="13">
+        <v>5.9580000000000002</v>
+      </c>
+      <c r="E19" s="13">
+        <v>5.9119999999999999</v>
+      </c>
+      <c r="F19" s="13">
+        <f>AVERAGE(B19:E19)</f>
+        <v>5.96</v>
+      </c>
+      <c r="G19" s="13">
+        <f>STDEV(B19:E19)</f>
+        <v>3.4525353003264328E-2</v>
+      </c>
+      <c r="H19" s="14">
+        <f t="shared" si="6"/>
+        <v>5.7928444636349543E-3</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="7"/>
+        <v>5.4937541051927184E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" s="13">
+        <v>5.984</v>
+      </c>
+      <c r="C20" s="13">
+        <v>5.952</v>
+      </c>
+      <c r="D20" s="13">
+        <v>5.8959999999999999</v>
+      </c>
+      <c r="E20" s="13">
+        <v>6.0819999999999999</v>
+      </c>
+      <c r="F20" s="13">
+        <f>AVERAGE(B20:E20)</f>
+        <v>5.9785000000000004</v>
+      </c>
+      <c r="G20" s="13">
+        <f>STDEV(B20:E20)</f>
+        <v>7.7997863218595045E-2</v>
+      </c>
+      <c r="H20" s="14">
+        <f t="shared" si="6"/>
+        <v>1.3046393446281683E-2</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="7"/>
+        <v>0.12411200581002095</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" s="13">
+        <v>5.931</v>
+      </c>
+      <c r="C21" s="13">
+        <v>5.92</v>
+      </c>
+      <c r="D21" s="13">
+        <v>5.8940000000000001</v>
+      </c>
+      <c r="E21" s="13">
+        <v>5.9050000000000002</v>
+      </c>
+      <c r="F21" s="13">
+        <f>AVERAGE(B21:E21)</f>
+        <v>5.9124999999999996</v>
+      </c>
+      <c r="G21" s="13">
+        <f>STDEV(B21:E21)</f>
+        <v>1.6299284237863455E-2</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="6"/>
+        <v>2.7567499768056587E-3</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="7"/>
+        <v>2.5935798450778775E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Checked various parallelization possibilities in Lanczos Algorithm and Hv; only one section worth parallelizing (Vv_5D_Composite_index). Now takes 55 percent of previous time.
</commit_message>
<xml_diff>
--- a/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
+++ b/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4940" yWindow="280" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="13440" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="117">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -330,6 +330,54 @@
   <si>
     <t>None (after):</t>
   </si>
+  <si>
+    <t>No Hv Parallelization:</t>
+  </si>
+  <si>
+    <t>Mv_5D_oneCompositeIndex</t>
+  </si>
+  <si>
+    <t>Mv_5D_oneCompositeIndex (no collapse)</t>
+  </si>
+  <si>
+    <t>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</t>
+  </si>
+  <si>
+    <t>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</t>
+  </si>
+  <si>
+    <t>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</t>
+  </si>
+  <si>
+    <t>Order of Execution:</t>
+  </si>
+  <si>
+    <t>diagMv_5D_oneCompositeIndex</t>
+  </si>
+  <si>
+    <t>calc_ulm</t>
+  </si>
+  <si>
+    <t>reshuffleIndices_5D_oneCompositeIndex</t>
+  </si>
+  <si>
+    <t>Hv_5D_oneCompositeIndex</t>
+  </si>
+  <si>
+    <t>Too long! Estimate is 2266s NOTE: this may not be a fair assessment as na and nb are only 2 and l_max =0</t>
+  </si>
+  <si>
+    <t>Need to check Cartesian grid generator with larger nx,ny,nz</t>
+  </si>
+  <si>
+    <t>Need to check calc_ulm, diagMv with larger na,nb, lmax</t>
+  </si>
+  <si>
+    <t>Need to check Hv_prep with larger system sizes</t>
+  </si>
+  <si>
+    <t>Need to check eliminating excess uec loops in lanczos algorithm</t>
+  </si>
 </sst>
 </file>
 
@@ -400,8 +448,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="259">
+  <cellStyleXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -682,7 +734,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="259">
+  <cellStyles count="263">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -812,6 +864,8 @@
     <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -941,6 +995,8 @@
     <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -984,24 +1040,28 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
           <c:errBars>
+            <c:errDir val="y"/>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
             <c:noEndCap val="1"/>
             <c:plus>
               <c:numRef>
-                <c:f>TimingLanczosParallelization!$I$14:$I$21</c:f>
+                <c:f>TimingLanczosParallelization!$J$14:$J$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>0.0417070485706302</c:v>
                   </c:pt>
@@ -1026,15 +1086,18 @@
                   <c:pt idx="7">
                     <c:v>0.0259357984507788</c:v>
                   </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.0732697357397158</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>TimingLanczosParallelization!$I$14:$I$21</c:f>
+                <c:f>TimingLanczosParallelization!$J$14:$J$22</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="8"/>
+                  <c:ptCount val="9"/>
                   <c:pt idx="0">
                     <c:v>0.0417070485706302</c:v>
                   </c:pt>
@@ -1059,15 +1122,18 @@
                   <c:pt idx="7">
                     <c:v>0.0259357984507788</c:v>
                   </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.0732697357397158</c:v>
+                  </c:pt>
                 </c:numCache>
               </c:numRef>
             </c:minus>
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>TimingLanczosParallelization!$A$14:$A$21</c:f>
+              <c:f>TimingLanczosParallelization!$B$14:$B$22</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>None:</c:v>
                 </c:pt>
@@ -1092,15 +1158,18 @@
                 <c:pt idx="7">
                   <c:v>None (after):</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>No Hv Parallelization:</c:v>
+                </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>TimingLanczosParallelization!$F$14:$F$21</c:f>
+              <c:f>TimingLanczosParallelization!$G$14:$G$22</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5.871</c:v>
                 </c:pt>
@@ -1125,9 +1194,13 @@
                 <c:pt idx="7">
                   <c:v>5.9125</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.04725</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1137,10 +1210,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="10"/>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="519670776"/>
         <c:axId val="571390920"/>
-      </c:barChart>
+      </c:lineChart>
       <c:catAx>
         <c:axId val="519670776"/>
         <c:scaling>
@@ -1162,6 +1236,7 @@
         <c:axId val="571390920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="4.9"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1206,20 +1281,228 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Effect of Collapse Directive on Vv_5D_Composite</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Index</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="1"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(TimingLanczosParallelization!$J$23,TimingLanczosParallelization!$J$26:$J$27)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0616688792220049</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0700921306050633</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0328296241330902</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(TimingLanczosParallelization!$J$23,TimingLanczosParallelization!$J$26:$J$27)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.0616688792220049</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.0700921306050633</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.0328296241330902</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>(TimingLanczosParallelization!$B$23,TimingLanczosParallelization!$B$26:$B$27)</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex (Collapse 3)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex(No Collapse)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Hv Critical Section: Vv_5D_CompositeIndex(Collapse 2)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(TimingLanczosParallelization!$G$23,TimingLanczosParallelization!$G$26:$G$27)</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.212</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.4185</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2905</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="763710872"/>
+        <c:axId val="649075272"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="763710872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="649075272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="649075272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="763710872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>203200</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1233,6 +1516,38 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -58705,20 +59020,20 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="B2" t="s">
         <v>85</v>
       </c>
@@ -58744,7 +59059,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -58774,7 +59089,7 @@
         <v>1.9013701042943409</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>84</v>
       </c>
@@ -58805,7 +59120,7 @@
         <v>2.574878340278715</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>92</v>
       </c>
@@ -58838,7 +59153,7 @@
         <v>1.1282258411168204</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -58871,7 +59186,7 @@
         <v>2.485911043364919</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="F7" s="13" t="e">
         <f t="shared" ref="F7:F10" si="3">AVERAGE(B7:D7)</f>
         <v>#DIV/0!</v>
@@ -58889,7 +59204,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="F8" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -58907,7 +59222,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="F9" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -58925,7 +59240,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="F10" s="13" t="e">
         <f t="shared" si="3"/>
         <v>#DIV/0!</v>
@@ -58943,299 +59258,681 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="B13" t="s">
+    <row r="13" spans="1:10">
+      <c r="C13" t="s">
         <v>85</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>87</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>94</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>88</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>90</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>89</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" t="s">
         <v>83</v>
       </c>
-      <c r="B14" s="13">
+      <c r="C14" s="13">
         <v>5.8490000000000002</v>
       </c>
-      <c r="C14" s="13">
+      <c r="D14" s="13">
         <v>5.9</v>
       </c>
-      <c r="D14" s="13">
+      <c r="E14" s="13">
         <v>5.8639999999999999</v>
       </c>
-      <c r="E14" s="13">
+      <c r="F14" s="13">
         <v>5.8470000000000004</v>
       </c>
-      <c r="F14" s="13">
-        <f>AVERAGE(B14:D14)</f>
+      <c r="G14" s="13">
+        <f>AVERAGE(C14:E14)</f>
         <v>5.8709999999999996</v>
       </c>
-      <c r="G14" s="13">
-        <f>STDEV(B14:D14)</f>
+      <c r="H14" s="13">
+        <f>STDEV(C14:E14)</f>
         <v>2.6210684844162443E-2</v>
       </c>
-      <c r="H14" s="14">
-        <f t="shared" ref="H14:H21" si="6">G14/F14</f>
+      <c r="I14" s="14">
+        <f t="shared" ref="I14:I21" si="6">H14/G14</f>
         <v>4.4644327787706425E-3</v>
       </c>
-      <c r="I14">
-        <f t="shared" ref="I14:I21" si="7">_xlfn.T.INV.2T(0.05, COUNT(B14:E14)-1)*G14/SQRT(COUNT(B14:E14))</f>
+      <c r="J14">
+        <f t="shared" ref="J14:J21" si="7">_xlfn.T.INV.2T(0.05, COUNT(C14:F14)-1)*H14/SQRT(COUNT(C14:F14))</f>
         <v>4.1707048570630241E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>84</v>
       </c>
-      <c r="B15" s="13">
+      <c r="C15" s="13">
         <v>6.1559999999999997</v>
       </c>
-      <c r="C15" s="13">
+      <c r="D15" s="13">
         <v>6.0369999999999999</v>
       </c>
-      <c r="D15" s="13">
+      <c r="E15" s="13">
         <v>5.931</v>
       </c>
-      <c r="E15" s="13">
+      <c r="F15" s="13">
         <v>5.9610000000000003</v>
       </c>
-      <c r="F15" s="13">
-        <f>AVERAGE(B15:E15)</f>
+      <c r="G15" s="13">
+        <f>AVERAGE(C15:F15)</f>
         <v>6.0212500000000002</v>
       </c>
-      <c r="G15" s="13">
-        <f>STDEV(B15:E15)</f>
+      <c r="H15" s="13">
+        <f>STDEV(C15:F15)</f>
         <v>0.1003007976040069</v>
       </c>
-      <c r="H15" s="14">
+      <c r="I15" s="14">
         <f t="shared" si="6"/>
         <v>1.6657803214283895E-2</v>
       </c>
-      <c r="I15">
+      <c r="J15">
         <f t="shared" si="7"/>
         <v>0.15960095137594044</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
         <v>92</v>
       </c>
-      <c r="B16" s="13">
+      <c r="C16" s="13">
         <v>5.8979999999999997</v>
       </c>
-      <c r="C16" s="13">
+      <c r="D16" s="13">
         <v>6.0620000000000003</v>
       </c>
-      <c r="D16" s="13">
+      <c r="E16" s="13">
         <v>5.9969999999999999</v>
       </c>
-      <c r="E16" s="13">
+      <c r="F16" s="13">
         <v>6.0380000000000003</v>
       </c>
-      <c r="F16" s="13">
-        <f>AVERAGE(B16:E16)</f>
+      <c r="G16" s="13">
+        <f>AVERAGE(C16:F16)</f>
         <v>5.9987500000000002</v>
       </c>
-      <c r="G16" s="13">
-        <f>STDEV(B16:E16)</f>
+      <c r="H16" s="13">
+        <f>STDEV(C16:F16)</f>
         <v>7.2329685007840122E-2</v>
       </c>
-      <c r="H16" s="14">
+      <c r="I16" s="14">
         <f t="shared" si="6"/>
         <v>1.2057459472030026E-2</v>
       </c>
-      <c r="I16">
+      <c r="J16">
         <f t="shared" si="7"/>
         <v>0.11509266940776765</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
+    <row r="17" spans="1:10">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
         <v>93</v>
       </c>
-      <c r="B17" s="13">
+      <c r="C17" s="13">
         <v>5.95</v>
       </c>
-      <c r="C17" s="13">
+      <c r="D17" s="13">
         <v>5.915</v>
       </c>
-      <c r="D17" s="13">
+      <c r="E17" s="13">
         <v>5.8920000000000003</v>
       </c>
-      <c r="E17" s="13">
+      <c r="F17" s="13">
         <v>5.8819999999999997</v>
       </c>
-      <c r="F17" s="13">
-        <f>AVERAGE(B17:E17)</f>
+      <c r="G17" s="13">
+        <f>AVERAGE(C17:F17)</f>
         <v>5.9097500000000007</v>
       </c>
-      <c r="G17" s="13">
-        <f>STDEV(B17:E17)</f>
+      <c r="H17" s="13">
+        <f>STDEV(C17:F17)</f>
         <v>3.018139603574814E-2</v>
       </c>
-      <c r="H17" s="14">
+      <c r="I17" s="14">
         <f t="shared" si="6"/>
         <v>5.1070512349504016E-3</v>
       </c>
-      <c r="I17">
+      <c r="J17">
         <f t="shared" si="7"/>
         <v>4.8025336151135523E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
+    <row r="18" spans="1:10">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
         <v>97</v>
       </c>
-      <c r="B18" s="13">
+      <c r="C18" s="13">
         <v>5.891</v>
       </c>
-      <c r="C18" s="13">
+      <c r="D18" s="13">
         <v>5.8890000000000002</v>
       </c>
-      <c r="D18" s="13">
+      <c r="E18" s="13">
         <v>5.8929999999999998</v>
       </c>
-      <c r="E18" s="13">
+      <c r="F18" s="13">
         <v>5.9020000000000001</v>
       </c>
-      <c r="F18" s="13">
-        <f>AVERAGE(B18:E18)</f>
+      <c r="G18" s="13">
+        <f>AVERAGE(C18:F18)</f>
         <v>5.8937500000000007</v>
       </c>
-      <c r="G18" s="13">
-        <f>STDEV(B18:E18)</f>
+      <c r="H18" s="13">
+        <f>STDEV(C18:F18)</f>
         <v>5.7373048260195084E-3</v>
       </c>
-      <c r="H18" s="14">
+      <c r="I18" s="14">
         <f t="shared" si="6"/>
         <v>9.7345574990786977E-4</v>
       </c>
-      <c r="I18">
+      <c r="J18">
         <f t="shared" si="7"/>
         <v>9.1293322729260884E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
+    <row r="19" spans="1:10">
+      <c r="A19">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
         <v>98</v>
       </c>
-      <c r="B19" s="13">
+      <c r="C19" s="13">
         <v>5.9820000000000002</v>
       </c>
-      <c r="C19" s="13">
+      <c r="D19" s="13">
         <v>5.9880000000000004</v>
       </c>
-      <c r="D19" s="13">
+      <c r="E19" s="13">
         <v>5.9580000000000002</v>
       </c>
-      <c r="E19" s="13">
+      <c r="F19" s="13">
         <v>5.9119999999999999</v>
       </c>
-      <c r="F19" s="13">
-        <f>AVERAGE(B19:E19)</f>
+      <c r="G19" s="13">
+        <f>AVERAGE(C19:F19)</f>
         <v>5.96</v>
       </c>
-      <c r="G19" s="13">
-        <f>STDEV(B19:E19)</f>
+      <c r="H19" s="13">
+        <f>STDEV(C19:F19)</f>
         <v>3.4525353003264328E-2</v>
       </c>
-      <c r="H19" s="14">
+      <c r="I19" s="14">
         <f t="shared" si="6"/>
         <v>5.7928444636349543E-3</v>
       </c>
-      <c r="I19">
+      <c r="J19">
         <f t="shared" si="7"/>
         <v>5.4937541051927184E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
-      <c r="A20" t="s">
+    <row r="20" spans="1:10">
+      <c r="A20">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
         <v>99</v>
       </c>
-      <c r="B20" s="13">
+      <c r="C20" s="13">
         <v>5.984</v>
       </c>
-      <c r="C20" s="13">
+      <c r="D20" s="13">
         <v>5.952</v>
       </c>
-      <c r="D20" s="13">
+      <c r="E20" s="13">
         <v>5.8959999999999999</v>
       </c>
-      <c r="E20" s="13">
+      <c r="F20" s="13">
         <v>6.0819999999999999</v>
       </c>
-      <c r="F20" s="13">
-        <f>AVERAGE(B20:E20)</f>
+      <c r="G20" s="13">
+        <f>AVERAGE(C20:F20)</f>
         <v>5.9785000000000004</v>
       </c>
-      <c r="G20" s="13">
-        <f>STDEV(B20:E20)</f>
+      <c r="H20" s="13">
+        <f>STDEV(C20:F20)</f>
         <v>7.7997863218595045E-2</v>
       </c>
-      <c r="H20" s="14">
+      <c r="I20" s="14">
         <f t="shared" si="6"/>
         <v>1.3046393446281683E-2</v>
       </c>
-      <c r="I20">
+      <c r="J20">
         <f t="shared" si="7"/>
         <v>0.12411200581002095</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
+    <row r="21" spans="1:10">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
         <v>100</v>
       </c>
-      <c r="B21" s="13">
+      <c r="C21" s="13">
         <v>5.931</v>
       </c>
-      <c r="C21" s="13">
+      <c r="D21" s="13">
         <v>5.92</v>
       </c>
-      <c r="D21" s="13">
+      <c r="E21" s="13">
         <v>5.8940000000000001</v>
       </c>
-      <c r="E21" s="13">
+      <c r="F21" s="13">
         <v>5.9050000000000002</v>
       </c>
-      <c r="F21" s="13">
-        <f>AVERAGE(B21:E21)</f>
+      <c r="G21" s="13">
+        <f>AVERAGE(C21:F21)</f>
         <v>5.9124999999999996</v>
       </c>
-      <c r="G21" s="13">
-        <f>STDEV(B21:E21)</f>
+      <c r="H21" s="13">
+        <f>STDEV(C21:F21)</f>
         <v>1.6299284237863455E-2</v>
       </c>
-      <c r="H21" s="14">
+      <c r="I21" s="14">
         <f t="shared" si="6"/>
         <v>2.7567499768056587E-3</v>
       </c>
-      <c r="I21">
+      <c r="J21">
         <f t="shared" si="7"/>
         <v>2.5935798450778775E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="13">
+        <v>4.9969999999999999</v>
+      </c>
+      <c r="D22" s="13">
+        <v>5.0529999999999999</v>
+      </c>
+      <c r="E22" s="13">
+        <v>5.032</v>
+      </c>
+      <c r="F22" s="13">
+        <v>5.1070000000000002</v>
+      </c>
+      <c r="G22" s="13">
+        <f t="shared" ref="G22:G28" si="8">AVERAGE(C22:F22)</f>
+        <v>5.04725</v>
+      </c>
+      <c r="H22" s="13">
+        <f t="shared" ref="H22:H28" si="9">STDEV(C22:F22)</f>
+        <v>4.6046172479371303E-2</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" ref="I22:I28" si="10">H22/G22</f>
+        <v>9.1230219385549163E-3</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ref="J22:J28" si="11">_xlfn.T.INV.2T(0.05, COUNT(C22:F22)-1)*H22/SQRT(COUNT(C22:F22))</f>
+        <v>7.3269735739715805E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
+      <c r="A23">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="13">
+        <v>3.16</v>
+      </c>
+      <c r="D23" s="13">
+        <v>3.2120000000000002</v>
+      </c>
+      <c r="E23" s="13">
+        <v>3.2530000000000001</v>
+      </c>
+      <c r="F23" s="13">
+        <v>3.2229999999999999</v>
+      </c>
+      <c r="G23" s="13">
+        <f t="shared" si="8"/>
+        <v>3.2119999999999997</v>
+      </c>
+      <c r="H23" s="13">
+        <f t="shared" si="9"/>
+        <v>3.8755644750152168E-2</v>
+      </c>
+      <c r="I23" s="14">
+        <f t="shared" si="10"/>
+        <v>1.2065891889835669E-2</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="11"/>
+        <v>6.1668879222004876E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C24" s="13">
+        <v>5.8170000000000002</v>
+      </c>
+      <c r="D24" s="13">
+        <v>5.8179999999999996</v>
+      </c>
+      <c r="E24" s="13">
+        <v>5.8479999999999999</v>
+      </c>
+      <c r="F24" s="13">
+        <v>5.8040000000000003</v>
+      </c>
+      <c r="G24" s="13">
+        <f t="shared" si="8"/>
+        <v>5.8217499999999998</v>
+      </c>
+      <c r="H24" s="13">
+        <f t="shared" si="9"/>
+        <v>1.8625699092025019E-2</v>
+      </c>
+      <c r="I24" s="14">
+        <f t="shared" si="10"/>
+        <v>3.1993299423755776E-3</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="11"/>
+        <v>2.9637643629370578E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="13">
+        <v>5.9909999999999997</v>
+      </c>
+      <c r="D25" s="13">
+        <v>5.9640000000000004</v>
+      </c>
+      <c r="E25" s="13">
+        <v>5.9630000000000001</v>
+      </c>
+      <c r="F25" s="13">
+        <v>6.024</v>
+      </c>
+      <c r="G25" s="13">
+        <f t="shared" si="8"/>
+        <v>5.9855</v>
+      </c>
+      <c r="H25" s="13">
+        <f t="shared" si="9"/>
+        <v>2.8757607689096677E-2</v>
+      </c>
+      <c r="I25" s="14">
+        <f t="shared" si="10"/>
+        <v>4.8045456000495659E-3</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="11"/>
+        <v>4.5759771169482051E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="13">
+        <v>3.403</v>
+      </c>
+      <c r="D26" s="13">
+        <v>3.3650000000000002</v>
+      </c>
+      <c r="E26" s="13">
+        <v>3.4660000000000002</v>
+      </c>
+      <c r="F26" s="13">
+        <v>3.44</v>
+      </c>
+      <c r="G26" s="13">
+        <f t="shared" si="8"/>
+        <v>3.4185000000000003</v>
+      </c>
+      <c r="H26" s="13">
+        <f t="shared" si="9"/>
+        <v>4.4049214900305896E-2</v>
+      </c>
+      <c r="I26" s="14">
+        <f t="shared" si="10"/>
+        <v>1.2885538949921279E-2</v>
+      </c>
+      <c r="J26">
+        <f t="shared" si="11"/>
+        <v>7.0092130605063308E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
+      <c r="A27">
+        <v>13</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" s="13">
+        <v>3.3109999999999999</v>
+      </c>
+      <c r="D27" s="13">
+        <v>3.262</v>
+      </c>
+      <c r="E27" s="13">
+        <v>3.2919999999999998</v>
+      </c>
+      <c r="F27" s="13">
+        <v>3.2970000000000002</v>
+      </c>
+      <c r="G27" s="13">
+        <f t="shared" si="8"/>
+        <v>3.2905000000000002</v>
+      </c>
+      <c r="H27" s="13">
+        <f t="shared" si="9"/>
+        <v>2.0631690833925031E-2</v>
+      </c>
+      <c r="I27" s="14">
+        <f t="shared" si="10"/>
+        <v>6.2700777492554413E-3</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="11"/>
+        <v>3.2829624133090242E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="13">
+        <v>5.8310000000000004</v>
+      </c>
+      <c r="D28" s="13">
+        <v>5.7990000000000004</v>
+      </c>
+      <c r="E28" s="13">
+        <v>5.8109999999999999</v>
+      </c>
+      <c r="F28" s="13">
+        <v>5.8860000000000001</v>
+      </c>
+      <c r="G28" s="13">
+        <f t="shared" si="8"/>
+        <v>5.8317500000000004</v>
+      </c>
+      <c r="H28" s="13">
+        <f t="shared" si="9"/>
+        <v>3.8499999999999958E-2</v>
+      </c>
+      <c r="I28" s="14">
+        <f t="shared" si="10"/>
+        <v>6.6017919149483351E-3</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="11"/>
+        <v>6.1262091376711333E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30">
+        <v>16</v>
+      </c>
+      <c r="B30" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="13">
+        <v>6.1120000000000001</v>
+      </c>
+      <c r="D30" s="13">
+        <v>6.1550000000000002</v>
+      </c>
+      <c r="E30" s="13">
+        <v>6.5460000000000003</v>
+      </c>
+      <c r="F30" s="13">
+        <v>6.2110000000000003</v>
+      </c>
+      <c r="G30" s="13">
+        <f t="shared" ref="G29:G31" si="12">AVERAGE(C30:F30)</f>
+        <v>6.2560000000000002</v>
+      </c>
+      <c r="H30" s="13">
+        <f t="shared" ref="H29:H31" si="13">STDEV(C30:F30)</f>
+        <v>0.19753649451852354</v>
+      </c>
+      <c r="I30" s="14">
+        <f t="shared" ref="I29:I31" si="14">H30/G30</f>
+        <v>3.1575526617411052E-2</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ref="J29:J31" si="15">_xlfn.T.INV.2T(0.05, COUNT(C30:F30)-1)*H30/SQRT(COUNT(C30:F30))</f>
+        <v>0.31432464356958545</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
+      <c r="A31">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="13">
+        <v>5.9320000000000004</v>
+      </c>
+      <c r="D31" s="13">
+        <v>5.8959999999999999</v>
+      </c>
+      <c r="E31" s="13">
+        <v>5.9020000000000001</v>
+      </c>
+      <c r="F31" s="13">
+        <v>5.9059999999999997</v>
+      </c>
+      <c r="G31" s="13">
+        <f t="shared" si="12"/>
+        <v>5.9089999999999998</v>
+      </c>
+      <c r="H31" s="13">
+        <f t="shared" si="13"/>
+        <v>1.5874507866387753E-2</v>
+      </c>
+      <c r="I31" s="14">
+        <f t="shared" si="14"/>
+        <v>2.6864965081042059E-3</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="15"/>
+        <v>2.5259884453791438E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Restored Coulomb Potential to working condition and running a job on Toby
</commit_message>
<xml_diff>
--- a/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
+++ b/Testing/FreeRotorExactCalc/Eigenvalues.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13440" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="13440" yWindow="500" windowWidth="25600" windowHeight="16060" tabRatio="500" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="TruncatedFreeParticle" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="118">
   <si>
     <t xml:space="preserve">H_bar = </t>
   </si>
@@ -377,6 +377,9 @@
   </si>
   <si>
     <t>Need to check eliminating excess uec loops in lanczos algorithm</t>
+  </si>
+  <si>
+    <t>Reactivate Coulomb Calc (with Vv parallelized)</t>
   </si>
 </sst>
 </file>
@@ -58311,7 +58314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:C81"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -59022,8 +59025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView showRuler="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -59863,19 +59866,19 @@
         <v>6.2110000000000003</v>
       </c>
       <c r="G30" s="13">
-        <f t="shared" ref="G29:G31" si="12">AVERAGE(C30:F30)</f>
+        <f t="shared" ref="G29:G32" si="12">AVERAGE(C30:F30)</f>
         <v>6.2560000000000002</v>
       </c>
       <c r="H30" s="13">
-        <f t="shared" ref="H29:H31" si="13">STDEV(C30:F30)</f>
+        <f t="shared" ref="H29:H32" si="13">STDEV(C30:F30)</f>
         <v>0.19753649451852354</v>
       </c>
       <c r="I30" s="14">
-        <f t="shared" ref="I29:I31" si="14">H30/G30</f>
+        <f t="shared" ref="I29:I32" si="14">H30/G30</f>
         <v>3.1575526617411052E-2</v>
       </c>
       <c r="J30">
-        <f t="shared" ref="J29:J31" si="15">_xlfn.T.INV.2T(0.05, COUNT(C30:F30)-1)*H30/SQRT(COUNT(C30:F30))</f>
+        <f t="shared" ref="J29:J32" si="15">_xlfn.T.INV.2T(0.05, COUNT(C30:F30)-1)*H30/SQRT(COUNT(C30:F30))</f>
         <v>0.31432464356958545</v>
       </c>
     </row>
@@ -59913,6 +59916,42 @@
       <c r="J31">
         <f t="shared" si="15"/>
         <v>2.5259884453791438E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
+      <c r="A32">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>117</v>
+      </c>
+      <c r="C32" s="13">
+        <v>6.7910000000000004</v>
+      </c>
+      <c r="D32" s="13">
+        <v>6.7350000000000003</v>
+      </c>
+      <c r="E32" s="13">
+        <v>6.6689999999999996</v>
+      </c>
+      <c r="F32" s="13">
+        <v>6.7469999999999999</v>
+      </c>
+      <c r="G32" s="13">
+        <f t="shared" si="12"/>
+        <v>6.7355</v>
+      </c>
+      <c r="H32" s="13">
+        <f t="shared" si="13"/>
+        <v>5.044799302251806E-2</v>
+      </c>
+      <c r="I32" s="14">
+        <f t="shared" si="14"/>
+        <v>7.4898660860393523E-3</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="15"/>
+        <v>8.0274014501745469E-2</v>
       </c>
     </row>
     <row r="34" spans="1:1">

</xml_diff>